<commit_message>
subiendo pruebas sprint II
</commit_message>
<xml_diff>
--- a/Testing/SpringII/TetsExploratorioSprintII.xlsx
+++ b/Testing/SpringII/TetsExploratorioSprintII.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yohana Zapata\OneDrive\Desktop\DIGH\ESPECIALIZACION BACK\PI\ecommerce-equipo4\Testing\SpringII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBE1F44-CF28-48C9-9E46-01E2F3254001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53783ECF-A6D7-4122-8B78-0822ABD973A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BG009" sheetId="11" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="71">
   <si>
     <t>COD</t>
   </si>
@@ -85,194 +85,197 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Validacion de campos de registro usuario</t>
-  </si>
-  <si>
     <t>Yohana Zapata</t>
   </si>
   <si>
     <t>Windows 11 / google chrome</t>
   </si>
   <si>
-    <t>Nayelly Pantoja</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
-    <t>Los campos de registrar usuario, en los datos de nombre y apellido permite formato de numeros, donde solo deberia de aceptar letras.</t>
-  </si>
-  <si>
-    <t>1. Abrir laaplicacion en http://localhost:5173/
-2. En la parte superior derecha dar clic en  crear cuenta
-3. Ingresar los datos</t>
-  </si>
-  <si>
-    <t>Que al ingresar numeros en el campo de nombre y apellido se muestre un aviso en rojo que diga que "no se permiten numeros".</t>
-  </si>
-  <si>
-    <t>Estos dos camor permite ingresar formato diferente a letras sin mostar el aviso y permite registrar el usuario.</t>
-  </si>
-  <si>
     <t>BG002</t>
   </si>
   <si>
-    <t>Redirigir a pagina principal despues de registro de usuario</t>
-  </si>
-  <si>
-    <t>Despues de registro de usuario no nos redirige a la pagina de inicio, se queda alli mostrando el formulario de registro.</t>
-  </si>
-  <si>
-    <t>1. Abrir laaplicacion en http://localhost:5173/
-2. En la parte superior derecha dar clic en  crear cuenta
-3. Ingresar los datos
-4. clic en boton registrarme</t>
-  </si>
-  <si>
-    <t>Cuando se realice el registro automaticamente nos redirija a la pagina de inicio de la aplicación.</t>
-  </si>
-  <si>
-    <t>Despues de registrarnos sale el aviso de registro exitoso y nos muestra nuevamente el formulario vacio, donde debemos quitarlo con la x del mismo.</t>
-  </si>
-  <si>
     <t>BG003</t>
   </si>
   <si>
-    <t>Buscador no tiene el filtro de servicio para realizar reserva</t>
-  </si>
-  <si>
-    <t>En el buscador no existe la opcion de filtrar los servicios que ofrece la categoria para realizar la reserva.</t>
-  </si>
-  <si>
-    <t>1. Abrir la aplicacion en http://localhost:5173/
-2. se muestra la pagina de inicio.</t>
-  </si>
-  <si>
-    <t>En la parte del buscador, cuando elegimos la categoria deberia estar el filtro de servicios para elegir el que se va a reservar.</t>
-  </si>
-  <si>
-    <t>No existe en el buscador la parte de servicios que tiene la categoria que se elige para reservar.</t>
-  </si>
-  <si>
     <t>BG004</t>
   </si>
   <si>
-    <t>Correo de validacio registro usuario nuevo</t>
-  </si>
-  <si>
     <t>Gonzalo Volante</t>
   </si>
   <si>
-    <t>Al registrarse como nuevo usuario se recibe un correo para autenticarse como usuario, no esta mostrardo los datos esperados.</t>
+    <t>Llegue un correo que muestre el nombre del usuario con los datos de fecha y hora actualizado, con ello el link de validacion de usuario.</t>
+  </si>
+  <si>
+    <t>Al resivir el correo llega y nos muestra el correo en vez del nombre del usuario, al igual que la hora incorrecta.</t>
+  </si>
+  <si>
+    <t>BG005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Espacios en pantalla de bienvenida usuario logeado </t>
+  </si>
+  <si>
+    <t>REPORTADO POR:</t>
+  </si>
+  <si>
+    <t>La pantalla de bienvenida  cuando un usuario se logea muestra una lectura personalizada que debe tener unos espacios entre el dato solicitado y los datos del usuario.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la pagina web.
+2. Dar clic en inicio de sesion.
+3. Diligenciar los datos.
+4. Aparace el recuadro de bienvenida.</t>
+  </si>
+  <si>
+    <t>Que aparezca en la ventana de bienvenida los datos y que estos tengan un espacios.</t>
+  </si>
+  <si>
+    <t>No cuenta con espacios entre los datos del formulario y los datos del usuario.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio de servicios es ambiguo </t>
+  </si>
+  <si>
+    <t>Se observa en la descripcion de los servicios el precio que no se especifica el valor real, pues tiene un signo de pesos pero no es coherente ya que muchos paises utilizan este signo para manejar su moneda.</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación.
+2. Seleccionar una categoria.
+3. Dar clic sobre la categoria.
+4. seleccionar un producto u dar clic sobre el.</t>
+  </si>
+  <si>
+    <t>Al seleccionar el producto queremos ver el valor real acorde al servicio y que nos especifique la moneda.</t>
+  </si>
+  <si>
+    <t>Que la estética y homogeneidad de las lista se encuentre correcta.</t>
+  </si>
+  <si>
+    <t>En la parte de descripción de un servicio estas poseen una lista, donde se encuentran con sus iniciales irregulares.</t>
+  </si>
+  <si>
+    <t>pasos para reproducción</t>
+  </si>
+  <si>
+    <t>1. Ingresar a la aplicación.
+2. Seleccionar una categoría.
+3. Dar clic sobre la categoría.
+4. seleccionar un producto y dar clic sobre el.</t>
+  </si>
+  <si>
+    <t>Se observa en la descripción de los servicios el precio que no se especifica el valor real, pues tiene un signo de pesos pero no es coherente ya que muchos países utilizan este signo para manejar su moneda.</t>
+  </si>
+  <si>
+    <t>iniciales de nombres de servicios con mayúscula y minúscula</t>
+  </si>
+  <si>
+    <t>Windows 11 / Google Chrome</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Asteriscos de campos obligatorios en formularios</t>
+  </si>
+  <si>
+    <t>Que los formularios contengas asteriscos para que el usuario visualmente ya sepa que son obligatorios.</t>
+  </si>
+  <si>
+    <t>En los formularios de registro e inicio de sesión debe haber unos asteriscos de campos obligatorios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ingresar a la aplicación.
+2. Dar clic en registro de usuario y/o inicio de sesión.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los formularios no tienen asteriscos para especificar que son obligatorios </t>
+  </si>
+  <si>
+    <t>Seguridad campo contraseña</t>
+  </si>
+  <si>
+    <t>La contraseña al ser unica debe contener una fuerte seguridad, por lo que debe contener variado formato de registro, como caracteres especiales, numeros y letras mayusculas y minusculas, adicional este campo debe contener un ojito que permita visualizar al usuario si lo prefiere cuando la esta ingresando para evitar errores.</t>
+  </si>
+  <si>
+    <t>Que la contraseña solicite un formato especial al registrar usuario y/o logeo, de igual forma que un ojito al dar clic sobre elpermita la visualizacion solo al usuario que se esta registrando o logeando.</t>
+  </si>
+  <si>
+    <t>El campo contraseña permite registrar usuario sin solicitar formato especial, tampoco posee un ojito para que el usuario pueda visualizar la contraseña y evitar errores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeronimo </t>
+  </si>
+  <si>
+    <t>Validacion Logo carrito de compras</t>
+  </si>
+  <si>
+    <t>El logo del carrito de compras es un símbolo integral en el comercio electrónico que facilita la interacción del consumidor con el sitio, mejora la experiencia de compra y contribuye a un proceso de compra más eficiente y agradable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Abrir laaplicacion en http://localhost:5173/carrito-de-compras
+2. En la parte superior derecha dice Carrito.
+</t>
+  </si>
+  <si>
+    <t>Encontrar el logo del carrito de compras.</t>
+  </si>
+  <si>
+    <t>Se encuentra la palabra Carrito</t>
+  </si>
+  <si>
+    <t>Separador de millares</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Se agragan productos al carrito de compras y se va a validar el valor a pagar.</t>
+  </si>
+  <si>
+    <t>Que los numeros esten en su orden ortografico correcto.</t>
+  </si>
+  <si>
+    <t>Se evidencian los numeros, perono cuentan con el separador de cifras o separador de millares.</t>
+  </si>
+  <si>
+    <t>Titulo de carro de compras</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El titulo de la pagina del carrito de compras debe ser mas acertado. </t>
   </si>
   <si>
     <t>1. Ingresar al sitio web.
 2. Dar clic sobre el formulario de registro 
 3. diligenciar formulario.
 . Dar clic en registrarme
-5. Ingresar al correo electronico que se registro en el formulario.
+5. Ingresar al correo electrónico que se registro en el formulario.
 6. Abrir correo en bandeja recibido de Hairphoria.</t>
   </si>
   <si>
-    <t>Llegue un correo que muestre el nombre del usuario con los datos de fecha y hora actualizado, con ello el link de validacion de usuario.</t>
-  </si>
-  <si>
-    <t>Al resivir el correo llega y nos muestra el correo en vez del nombre del usuario, al igual que la hora incorrecta.</t>
-  </si>
-  <si>
-    <t>BG005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Espacios en pantalla de bienvenida usuario logeado </t>
-  </si>
-  <si>
-    <t>REPORTADO POR:</t>
-  </si>
-  <si>
-    <t>La pantalla de bienvenida  cuando un usuario se logea muestra una lectura personalizada que debe tener unos espacios entre el dato solicitado y los datos del usuario.</t>
-  </si>
-  <si>
-    <t>1. Ingresar a la pagina web.
-2. Dar clic en inicio de sesion.
-3. Diligenciar los datos.
-4. Aparace el recuadro de bienvenida.</t>
-  </si>
-  <si>
-    <t>Que aparezca en la ventana de bienvenida los datos y que estos tengan un espacios.</t>
-  </si>
-  <si>
-    <t>No cuenta con espacios entre los datos del formulario y los datos del usuario.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Precio de servicios es ambiguo </t>
-  </si>
-  <si>
-    <t>Se observa en la descripcion de los servicios el precio que no se especifica el valor real, pues tiene un signo de pesos pero no es coherente ya que muchos paises utilizan este signo para manejar su moneda.</t>
-  </si>
-  <si>
-    <t>1. Ingresar a la aplicación.
-2. Seleccionar una categoria.
-3. Dar clic sobre la categoria.
-4. seleccionar un producto u dar clic sobre el.</t>
-  </si>
-  <si>
-    <t>Al seleccionar el producto queremos ver el valor real acorde al servicio y que nos especifique la moneda.</t>
-  </si>
-  <si>
-    <t>Que la estética y homogeneidad de las lista se encuentre correcta.</t>
-  </si>
-  <si>
-    <t>En la parte de descripción de un servicio estas poseen una lista, donde se encuentran con sus iniciales irregulares.</t>
-  </si>
-  <si>
-    <t>pasos para reproducción</t>
-  </si>
-  <si>
-    <t>1. Ingresar a la aplicación.
-2. Seleccionar una categoría.
-3. Dar clic sobre la categoría.
-4. seleccionar un producto y dar clic sobre el.</t>
-  </si>
-  <si>
-    <t>Se observa en la descripción de los servicios el precio que no se especifica el valor real, pues tiene un signo de pesos pero no es coherente ya que muchos países utilizan este signo para manejar su moneda.</t>
-  </si>
-  <si>
-    <t>iniciales de nombres de servicios con mayúscula y minúscula</t>
-  </si>
-  <si>
-    <t>Windows 11 / Google Chrome</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Asteriscos de campos obligatorios en formularios</t>
-  </si>
-  <si>
-    <t>Que los formularios contengas asteriscos para que el usuario visualmente ya sepa que son obligatorios.</t>
-  </si>
-  <si>
-    <t>En los formularios de registro e inicio de sesión debe haber unos asteriscos de campos obligatorios.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ingresar a la aplicación.
-2. Dar clic en registro de usuario y/o inicio de sesión.
+    <t>Validacion de asentos y puntuacion.</t>
+  </si>
+  <si>
+    <t>Jeronimo</t>
+  </si>
+  <si>
+    <t>Se evidencia que los asentos y puntuacion faltan en agunas partes de la pagina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Abrir laaplicacion en http://localhost:5173/carrito-de-compras
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Los formularios no tienen asteriscos para especificar que son obligatorios </t>
-  </si>
-  <si>
-    <t>Seguridad campo contraseña</t>
-  </si>
-  <si>
-    <t>La contraseña al ser unica debe contener una fuerte seguridad, por lo que debe contener variado formato de registro, como caracteres especiales, numeros y letras mayusculas y minusculas, adicional este campo debe contener un ojito que permita visualizar al usuario si lo prefiere cuando la esta ingresando para evitar errores.</t>
-  </si>
-  <si>
-    <t>Que la contraseña solicite un formato especial al registrar usuario y/o logeo, de igual forma que un ojito al dar clic sobre elpermita la visualizacion solo al usuario que se esta registrando o logeando.</t>
-  </si>
-  <si>
-    <t>El campo contraseña permite registrar usuario sin solicitar formato especial, tampoco posee un ojito para que el usuario pueda visualizar la contraseña y evitar errores.</t>
+    <t xml:space="preserve">Que todo este de acuerdo a su ortografia y puntiacion. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faltan los acentos y puntos. </t>
   </si>
 </sst>
 </file>
@@ -648,45 +651,45 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,6 +723,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -738,7 +744,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,12 +763,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1117,22 +1120,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>64010</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2505075</xdr:colOff>
+      <xdr:colOff>2644775</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>892995</xdr:rowOff>
+      <xdr:rowOff>921924</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
+        <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2DB2668-9039-02CD-DE67-B0D0612EC23D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9FD36AA-D476-1881-6960-153244A58329}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1148,8 +1151,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2209801" y="6588635"/>
-          <a:ext cx="2263774" cy="1733860"/>
+          <a:off x="2495550" y="6810375"/>
+          <a:ext cx="2120900" cy="1772824"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1165,23 +1168,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1051134</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400052</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3423037</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>2921000</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1914D35-2C6D-E6D4-FA75-489F2D48EAA7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E6BC34-5A70-B40C-90EB-EC39EFA7B6B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1197,8 +1200,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1857584" y="6673851"/>
-          <a:ext cx="3533953" cy="1308099"/>
+          <a:off x="2371727" y="6619875"/>
+          <a:ext cx="2524123" cy="1019175"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1215,22 +1218,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:colOff>390526</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>25401</xdr:rowOff>
+      <xdr:rowOff>130175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3620107</xdr:colOff>
+      <xdr:colOff>4267444</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>901209</xdr:rowOff>
+      <xdr:rowOff>952500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67882F7A-3AC2-73EB-2B06-71608F3F384A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{282C16DF-7C04-AC80-ACD6-272555EC9FDA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1246,8 +1249,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1835150" y="6661151"/>
-          <a:ext cx="3753457" cy="1796558"/>
+          <a:off x="1200151" y="6711950"/>
+          <a:ext cx="5038968" cy="1727200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1264,22 +1267,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>882650</xdr:colOff>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>43682</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2552700</xdr:colOff>
+      <xdr:colOff>2609850</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>520282</xdr:rowOff>
+      <xdr:rowOff>496928</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="5" name="Imagen 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E18FAAB0-FDA1-421F-D3C5-2FECD824E47C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A4BF66A-CCE7-CE7F-E5EF-86E0171BA14E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1295,8 +1298,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2978150" y="7136632"/>
-          <a:ext cx="1670050" cy="1460850"/>
+          <a:off x="2409825" y="7210424"/>
+          <a:ext cx="2295525" cy="1487529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1634,7 +1637,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -1644,17 +1647,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -1674,7 +1677,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -1684,7 +1687,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -1694,7 +1697,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -1706,212 +1709,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="39"/>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="39"/>
+      <c r="C17" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -1928,17 +1931,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1977,7 +1980,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -1987,17 +1990,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -2017,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -2027,7 +2030,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -2037,7 +2040,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -2049,212 +2052,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="39"/>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="39"/>
+      <c r="C17" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -2271,17 +2274,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2320,7 +2323,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -2330,17 +2333,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -2360,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -2370,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -2380,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -2392,212 +2395,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="39"/>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="39"/>
+      <c r="C17" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -2614,17 +2617,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2663,7 +2666,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -2673,17 +2676,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -2703,7 +2706,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -2713,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -2723,7 +2726,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -2735,212 +2738,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -2957,17 +2960,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3006,7 +3009,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="E3" s="19"/>
     </row>
@@ -3016,17 +3019,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="E4" s="19"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="17"/>
       <c r="C5" s="36" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="19"/>
     </row>
@@ -3046,7 +3049,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="19"/>
     </row>
@@ -3056,7 +3059,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E8" s="19"/>
     </row>
@@ -3066,7 +3069,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="19"/>
     </row>
@@ -3086,34 +3089,34 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="17"/>
-      <c r="C12" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="19"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="17"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="17"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="17"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="17"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="19"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
@@ -3126,34 +3129,34 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="17"/>
-      <c r="C18" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="19"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="17"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="19"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="17"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="19"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="17"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="19"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="17"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="19"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
@@ -3166,34 +3169,34 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="17"/>
-      <c r="C24" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="19"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="17"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="19"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="17"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="19"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="17"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="19"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="17"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="19"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
@@ -3206,40 +3209,40 @@
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="17"/>
-      <c r="C30" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="47"/>
+      <c r="C30" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="46"/>
       <c r="E30" s="19"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="17"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="19"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="17"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49"/>
+      <c r="C32" s="47"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="19"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="17"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="19"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="17"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="49"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="19"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="17"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="50"/>
       <c r="E35" s="19"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
@@ -3300,17 +3303,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3322,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3349,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -3359,17 +3362,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -3379,7 +3382,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="30">
-        <v>45079</v>
+        <v>45440</v>
       </c>
       <c r="E6" s="29"/>
     </row>
@@ -3389,7 +3392,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -3399,7 +3402,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -3409,7 +3412,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -3421,212 +3424,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="39"/>
+      <c r="C11" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="39"/>
+      <c r="C17" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="46"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" ht="28" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -3643,17 +3646,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3663,10 +3666,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="B1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3692,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -3702,17 +3708,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
       <c r="C5" s="34" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -3722,7 +3728,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="30">
-        <v>45077</v>
+        <v>45440</v>
       </c>
       <c r="E6" s="29"/>
     </row>
@@ -3732,7 +3738,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -3742,7 +3748,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -3752,7 +3758,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -3764,212 +3770,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="72"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="74"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="41"/>
+      <c r="C24" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -3986,17 +3992,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4008,8 +4014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4035,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E3" s="29"/>
     </row>
@@ -4045,17 +4051,15 @@
         <v>1</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="27"/>
-      <c r="C5" s="34" t="s">
-        <v>43</v>
-      </c>
+      <c r="C5" s="34"/>
       <c r="D5" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="29"/>
     </row>
@@ -4065,7 +4069,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="30">
-        <v>45077</v>
+        <v>45440</v>
       </c>
       <c r="E6" s="29"/>
     </row>
@@ -4075,7 +4079,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="29"/>
     </row>
@@ -4085,7 +4089,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="E8" s="29"/>
     </row>
@@ -4095,7 +4099,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="29"/>
     </row>
@@ -4107,212 +4111,212 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="27"/>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="29"/>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="27"/>
-      <c r="C12" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="41"/>
+      <c r="C12" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="40"/>
       <c r="E12" s="29"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="27"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
       <c r="E13" s="29"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="27"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
       <c r="E14" s="29"/>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="27"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="29"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="27"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="45"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="27"/>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="45"/>
       <c r="E17" s="29"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="27"/>
-      <c r="C18" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="47"/>
+      <c r="C18" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="72"/>
       <c r="E18" s="29"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="27"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="49"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
       <c r="E19" s="29"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="29"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="27"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="74"/>
       <c r="E21" s="29"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="27"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="29"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="27"/>
-      <c r="C23" s="39" t="s">
+      <c r="C23" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="29"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="27"/>
-      <c r="C24" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="47"/>
+      <c r="C24" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="46"/>
       <c r="E24" s="29"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="27"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="29"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="27"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="49"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="29"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="27"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="49"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="29"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="27"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="51"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="29"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="27"/>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="45"/>
       <c r="E29" s="29"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="27"/>
-      <c r="C30" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="41"/>
+      <c r="C30" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="40"/>
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="43"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="29"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="27"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="43"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="27"/>
-      <c r="C33" s="42"/>
-      <c r="D33" s="43"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
       <c r="E33" s="29"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="27"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="27"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="29"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="27"/>
-      <c r="C36" s="39" t="s">
+      <c r="C36" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="39"/>
+      <c r="D36" s="45"/>
       <c r="E36" s="29"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="27"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="46"/>
       <c r="E37" s="29"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="27"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="49"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="29"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="27"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="49"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
       <c r="E39" s="29"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="27"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
       <c r="E40" s="29"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="27"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="49"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="2:5" ht="77" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="27"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="51"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="29"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
@@ -4329,17 +4333,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4351,8 +4355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4388,17 +4392,17 @@
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="8"/>
     </row>
@@ -4408,7 +4412,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="9">
-        <v>45077</v>
+        <v>45440</v>
       </c>
       <c r="E6" s="8"/>
     </row>
@@ -4418,7 +4422,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="8"/>
     </row>
@@ -4428,7 +4432,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -4438,7 +4442,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -4450,218 +4454,218 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="6"/>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="69"/>
+      <c r="D11" s="63"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
-      <c r="C12" s="63" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="64"/>
+      <c r="C12" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="65"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="6"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="67"/>
       <c r="E13" s="8"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B14" s="6"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="67"/>
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B15" s="6"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B16" s="6"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" s="6"/>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="69"/>
+      <c r="D17" s="63"/>
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
-      <c r="C18" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="70"/>
+      <c r="C18" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="72"/>
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="6"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="72"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="74"/>
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="74"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="6"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="74"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="6"/>
-      <c r="C23" s="69" t="s">
+      <c r="C23" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="69"/>
+      <c r="D23" s="63"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
-      <c r="C24" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="64"/>
+      <c r="C24" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="65"/>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" s="6"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="67"/>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" s="6"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="68"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="69"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="6"/>
-      <c r="C29" s="69" t="s">
+      <c r="C29" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="69"/>
+      <c r="D29" s="63"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="6"/>
-      <c r="C30" s="63" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="64"/>
+      <c r="C30" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="65"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="6"/>
-      <c r="C31" s="65"/>
-      <c r="D31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="67"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="6"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="67"/>
       <c r="E32" s="8"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" s="6"/>
-      <c r="C33" s="65"/>
-      <c r="D33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="67"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="6"/>
-      <c r="C34" s="65"/>
-      <c r="D34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="67"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="6"/>
-      <c r="C36" s="69" t="s">
+      <c r="C36" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="69"/>
+      <c r="D36" s="63"/>
       <c r="E36" s="8"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="6"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
       <c r="E37" s="8"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
-      <c r="C38" s="65"/>
-      <c r="D38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="67"/>
       <c r="E38" s="8"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="67"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" s="6"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="67"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="6"/>
-      <c r="C41" s="65"/>
-      <c r="D41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="2:5" ht="41" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="69"/>
       <c r="E42" s="8"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="6"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="76"/>
+      <c r="C43" s="70"/>
+      <c r="D43" s="71"/>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
@@ -4672,17 +4676,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D42"/>
-    <mergeCell ref="C43:D43"/>
     <mergeCell ref="C24:D28"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D22"/>
     <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D42"/>
+    <mergeCell ref="C43:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>